<commit_message>
Update 04/08/2022 : New image (png)
</commit_message>
<xml_diff>
--- a/data/dataLOOP.xlsx
+++ b/data/dataLOOP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="159">
   <si>
     <t>spplat</t>
   </si>
@@ -531,7 +531,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -576,11 +576,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -588,6 +619,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,8 +640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D37" totalsRowShown="0">
-  <autoFilter ref="A1:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D69" totalsRowShown="0">
+  <autoFilter ref="A1:D69"/>
   <sortState ref="A2:D31">
     <sortCondition ref="A1:A31"/>
   </sortState>
@@ -884,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,6 +1450,454 @@
         <v>11</v>
       </c>
     </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1428,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update 09/08/2022 : New output directory
</commit_message>
<xml_diff>
--- a/data/dataLOOP.xlsx
+++ b/data/dataLOOP.xlsx
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,518 +947,518 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B29" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D29" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D30" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B31" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D31" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B32" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B33" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D33" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B34" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D34" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B35" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D35" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B36" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C36" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D36" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>148</v>
-      </c>
-      <c r="B22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>151</v>
-      </c>
-      <c r="B25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>154</v>
-      </c>
-      <c r="B36" t="s">
-        <v>155</v>
-      </c>
-      <c r="C36" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="D37" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>10</v>
@@ -1466,13 +1466,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>11</v>
@@ -1480,13 +1480,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>10</v>
@@ -1494,13 +1494,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>11</v>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>10</v>
@@ -1522,13 +1522,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>11</v>
@@ -1536,27 +1536,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>7</v>
+        <v>143</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>9</v>
+      <c r="A45" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>11</v>
@@ -1564,27 +1564,27 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>50</v>
+      <c r="A47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>11</v>
@@ -1592,13 +1592,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>10</v>
@@ -1606,13 +1606,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>11</v>
@@ -1620,13 +1620,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>10</v>
@@ -1634,13 +1634,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>8</v>
+        <v>152</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>11</v>
@@ -1648,13 +1648,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>10</v>
@@ -1662,13 +1662,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>11</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>10</v>
@@ -1690,13 +1690,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>11</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>10</v>
@@ -1718,13 +1718,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>11</v>
@@ -1732,13 +1732,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>10</v>
@@ -1746,13 +1746,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>11</v>
@@ -1760,13 +1760,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>10</v>
@@ -1774,13 +1774,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>11</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>34</v>
+        <v>155</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>10</v>
@@ -1802,13 +1802,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>34</v>
+        <v>155</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>11</v>
@@ -1816,13 +1816,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>10</v>
@@ -1830,13 +1830,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>11</v>
@@ -1844,13 +1844,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>10</v>
@@ -1858,13 +1858,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>11</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>10</v>
@@ -1886,13 +1886,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>11</v>
@@ -1910,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update 12/09/2022: New photos update
</commit_message>
<xml_diff>
--- a/data/dataLOOP.xlsx
+++ b/data/dataLOOP.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="108">
   <si>
     <t>spplat</t>
   </si>
@@ -349,15 +348,6 @@
   </si>
   <si>
     <t>Sériole limon</t>
-  </si>
-  <si>
-    <t>Anisotremus surinamensis</t>
-  </si>
-  <si>
-    <t>Black margate</t>
-  </si>
-  <si>
-    <t>Lippu croupia</t>
   </si>
 </sst>
 </file>
@@ -496,8 +486,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D73" totalsRowShown="0">
-  <autoFilter ref="A1:D73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D71" totalsRowShown="0">
+  <autoFilter ref="A1:D71"/>
   <sortState ref="A2:D69">
     <sortCondition ref="A1:A69"/>
   </sortState>
@@ -774,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:D73"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,81 +1743,38 @@
         <v>11</v>
       </c>
     </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 14/09/2022 : dataset update
</commit_message>
<xml_diff>
--- a/data/dataLOOP.xlsx
+++ b/data/dataLOOP.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="108">
   <si>
     <t>spplat</t>
   </si>
@@ -457,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -468,6 +469,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,4 +1779,999 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 10/07/2023 : MED files
</commit_message>
<xml_diff>
--- a/data/dataLOOP.xlsx
+++ b/data/dataLOOP.xlsx
@@ -396,18 +396,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -425,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -470,31 +464,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -502,14 +476,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -637,10 +639,10 @@
     <sortCondition ref="A1:A69"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="spplat" dataDxfId="2"/>
-    <tableColumn id="2" name="sppeng" dataDxfId="1"/>
-    <tableColumn id="3" name="sppfr" dataDxfId="0"/>
-    <tableColumn id="4" name="sex"/>
+    <tableColumn id="1" name="spplat" dataDxfId="3"/>
+    <tableColumn id="2" name="sppeng" dataDxfId="2"/>
+    <tableColumn id="3" name="sppfr" dataDxfId="1"/>
+    <tableColumn id="4" name="sex" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -911,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D81" sqref="A72:D81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,142 +1919,142 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D74" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="C76" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D76" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D77" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C79" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D80" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>